<commit_message>
IRAS of SnNi plots
</commit_message>
<xml_diff>
--- a/plotTPD_data programs/HOAc Area_output.xlsx
+++ b/plotTPD_data programs/HOAc Area_output.xlsx
@@ -14,39 +14,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>HOAc</t>
+  </si>
   <si>
     <t>14</t>
   </si>
   <si>
-    <t>CH4</t>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>Formaldehyde</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>Water</t>
   </si>
   <si>
     <t>31-ol</t>
   </si>
   <si>
-    <t>Formaldehyde</t>
-  </si>
-  <si>
-    <t>27-eth</t>
-  </si>
-  <si>
-    <t>HOAc</t>
-  </si>
-  <si>
-    <t>CO</t>
-  </si>
-  <si>
-    <t>H2</t>
-  </si>
-  <si>
-    <t>Water</t>
-  </si>
-  <si>
     <t>CO2</t>
-  </si>
-  <si>
-    <t>L</t>
   </si>
 </sst>
 </file>
@@ -404,16 +398,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="1" t="s">
-        <v>10</v>
-      </c>
+    <row r="1" spans="1:10">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -441,11 +432,8 @@
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -456,133 +444,25 @@
         <v>-1</v>
       </c>
       <c r="D2">
-        <v>-1</v>
+        <v>1607318.565012615</v>
       </c>
       <c r="E2">
         <v>-1</v>
       </c>
       <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>60978.88933325125</v>
+      </c>
+      <c r="H2">
         <v>-1</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>-1</v>
       </c>
-      <c r="H2">
-        <v>51218.63938013145</v>
-      </c>
-      <c r="I2">
-        <v>153794.7478142115</v>
-      </c>
       <c r="J2">
-        <v>-1</v>
-      </c>
-      <c r="K2">
-        <v>37458.77268615671</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="1">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>-1</v>
-      </c>
-      <c r="C3">
-        <v>-1</v>
-      </c>
-      <c r="D3">
-        <v>-1</v>
-      </c>
-      <c r="E3">
-        <v>-1</v>
-      </c>
-      <c r="F3">
-        <v>-1</v>
-      </c>
-      <c r="G3">
-        <v>-1</v>
-      </c>
-      <c r="H3">
-        <v>60895.45292703531</v>
-      </c>
-      <c r="I3">
-        <v>1349353.689874392</v>
-      </c>
-      <c r="J3">
-        <v>-1</v>
-      </c>
-      <c r="K3">
-        <v>282216.8310418345</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="1">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>-1</v>
-      </c>
-      <c r="C4">
-        <v>-1</v>
-      </c>
-      <c r="D4">
-        <v>-1</v>
-      </c>
-      <c r="E4">
-        <v>-1</v>
-      </c>
-      <c r="F4">
-        <v>-1</v>
-      </c>
-      <c r="G4">
-        <v>-1</v>
-      </c>
-      <c r="H4">
-        <v>42382.16126869109</v>
-      </c>
-      <c r="I4">
-        <v>192271.0642769816</v>
-      </c>
-      <c r="J4">
-        <v>-1</v>
-      </c>
-      <c r="K4">
-        <v>70768.42674768422</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="1">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>-1</v>
-      </c>
-      <c r="C5">
-        <v>-1</v>
-      </c>
-      <c r="D5">
-        <v>-1</v>
-      </c>
-      <c r="E5">
-        <v>-1</v>
-      </c>
-      <c r="F5">
-        <v>-1</v>
-      </c>
-      <c r="G5">
-        <v>-1</v>
-      </c>
-      <c r="H5">
-        <v>41877.98208514423</v>
-      </c>
-      <c r="I5">
-        <v>170221.4798536748</v>
-      </c>
-      <c r="J5">
-        <v>-1</v>
-      </c>
-      <c r="K5">
-        <v>33416.59657643169</v>
+        <v>282318.2582178094</v>
       </c>
     </row>
   </sheetData>

</xml_diff>